<commit_message>
evolutionary strategy with analysis finished
</commit_message>
<xml_diff>
--- a/analysis/statistics/statistical_analysis.xlsx
+++ b/analysis/statistics/statistical_analysis.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="hypothesis_test" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="anova" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,17 +473,17 @@
         <v>508.72</v>
       </c>
       <c r="C2" t="n">
-        <v>504.77</v>
+        <v>504.81</v>
       </c>
       <c r="D2" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0012</v>
+        <v>0.4563</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mann-Whitney U</t>
+          <t>t-test (1-sample)</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -506,13 +505,13 @@
         <v>641.67</v>
       </c>
       <c r="C3" t="n">
-        <v>562.8200000000001</v>
+        <v>562.66</v>
       </c>
       <c r="D3" t="n">
-        <v>1.12</v>
+        <v>1.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -538,17 +537,17 @@
         <v>546.88</v>
       </c>
       <c r="C4" t="n">
-        <v>541.5</v>
+        <v>541.52</v>
       </c>
       <c r="D4" t="n">
-        <v>0.25</v>
+        <v>0.28</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0426</v>
+        <v>0.2704</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mann-Whitney U</t>
+          <t>t-test (1-sample)</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -570,17 +569,17 @@
         <v>631.05</v>
       </c>
       <c r="C5" t="n">
-        <v>591.41</v>
+        <v>591.03</v>
       </c>
       <c r="D5" t="n">
-        <v>1.77</v>
+        <v>1.54</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0018</v>
+        <v>0.978</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Mann-Whitney U</t>
+          <t>t-test (1-sample)</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -602,13 +601,13 @@
         <v>532.41</v>
       </c>
       <c r="C6" t="n">
-        <v>522.59</v>
+        <v>522.38</v>
       </c>
       <c r="D6" t="n">
-        <v>0.32</v>
+        <v>0.29</v>
       </c>
       <c r="E6" t="n">
-        <v>0.604</v>
+        <v>0.3609</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -634,17 +633,17 @@
         <v>670.96</v>
       </c>
       <c r="C7" t="n">
-        <v>599.52</v>
+        <v>598.92</v>
       </c>
       <c r="D7" t="n">
-        <v>3.63</v>
+        <v>2.91</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3958</v>
+        <v>0.0476</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>t-test (1-sample)</t>
+          <t>Mann-Whitney U</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -653,64 +652,6 @@
       <c r="H7" t="inlineStr">
         <is>
           <t>reject H0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>anova_across_instances</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>F-statistic</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>14424.65232726994</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>p-value</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>9.496497498097145e-226</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>result</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>significant differences</t>
         </is>
       </c>
     </row>

</xml_diff>